<commit_message>
ignore excel file type
</commit_message>
<xml_diff>
--- a/WebScrapingNetwork/website&ip.xlsx
+++ b/WebScrapingNetwork/website&ip.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,103 +453,251 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>142.251.220.13\\n</t>
+          <t xml:space="preserve">142.251.130.13
+</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>www.baidu.com</t>
+          <t>www.126.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>183.2.172.185\\n183.2.172.42\\n</t>
+          <t xml:space="preserve">220.181.72.180
+</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dss0.bdstatic.com</t>
+          <t>urswebzj.nosdn.127.net</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>39.91.182.33\\n</t>
+          <t xml:space="preserve">119.188.91.244
+119.188.91.241
+119.167.137.106
+119.167.137.102
+119.167.137.105
+119.188.91.242
+119.188.91.238
+119.188.91.243
+</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>pss.bdstatic.com</t>
+          <t>mimg.127.net</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>112.84.34.36\\n</t>
+          <t xml:space="preserve">61.170.81.231
+61.170.81.215
+61.170.81.250
+</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hectorstatic.baidu.com</t>
+          <t>dl.reg.163.com</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>117.68.52.38\\n122.228.115.38\\n</t>
+          <t xml:space="preserve">223.252.215.2
+</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sp1.baidu.com</t>
+          <t>passport.126.com</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>183.2.172.42\\n183.2.172.185\\n</t>
+          <t xml:space="preserve">223.252.215.4
+</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>hector.baidu.com</t>
+          <t>onegoods.nosdn.127.net</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>39.156.68.81\\n</t>
+          <t xml:space="preserve">119.188.91.238
+119.188.91.223
+119.188.91.237
+119.188.91.241
+119.167.137.74
+119.167.137.101
+119.188.91.224
+119.167.137.75
+</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>sp2.baidu.com</t>
+          <t>utility.mail.163.com</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>183.2.172.42\\n183.2.172.185\\n</t>
+          <t xml:space="preserve">220.181.12.191
+</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>mail.126.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">123.126.96.204
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>countly.mail.163.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">111.124.200.205
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>cstaticdun.126.net</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">183.2.193.244
+183.2.193.238
+14.119.65.239
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>fl.reg.163.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59.111.160.204
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>content-autofill.googleapis.com</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>216.58.203.74\\n142.251.220.10\\n142.250.207.74\\n172.217.24.106\\n172.217.24.234\\n172.217.25.10\\n172.217.27.10\\n172.217.27.42\\n172.217.31.10\\n142.250.199.74\\n142.250.204.42\\n142.250.204.74\\n142.250.204.106\\n142.250.204.138\\n172.217.24.74\\n216.58.200.234\\n</t>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">172.217.27.10
+172.217.27.42
+172.217.31.10
+142.250.199.74
+142.250.204.42
+142.250.204.74
+142.251.130.10
+142.251.222.202
+142.250.66.42
+142.250.66.74
+142.250.66.106
+142.250.66.138
+142.250.207.74
+172.217.24.106
+172.217.24.234
+172.217.25.10
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>pr.nss.netease.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">59.111.160.244
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mail-activity.nosdn.127.net</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">183.2.193.243
+183.2.193.248
+183.2.193.238
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>b.mail.126.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">220.181.12.191
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mail.163.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">220.181.12.133
+</t>
         </is>
       </c>
     </row>

</xml_diff>